<commit_message>
Update on Michael Laptop
</commit_message>
<xml_diff>
--- a/StudentSchedules.xlsx
+++ b/StudentSchedules.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="114">
   <si>
     <t>R-Number</t>
   </si>
@@ -149,16 +149,16 @@
     <t>08:00-08:50A</t>
   </si>
   <si>
-    <t>91745</t>
-  </si>
-  <si>
-    <t>RCC 100 26</t>
-  </si>
-  <si>
-    <t>Experiments in Psychology</t>
-  </si>
-  <si>
-    <t>09:30-10:45A</t>
+    <t>91723</t>
+  </si>
+  <si>
+    <t>RCC 100 04</t>
+  </si>
+  <si>
+    <t>Strengthening Roots Stem Success</t>
+  </si>
+  <si>
+    <t>09:00-09:50A</t>
   </si>
   <si>
     <t>Tim Johnson</t>
@@ -167,13 +167,199 @@
     <t>R00000002</t>
   </si>
   <si>
-    <t>92180</t>
-  </si>
-  <si>
-    <t>ENG 234</t>
-  </si>
-  <si>
-    <t>Literature and Law</t>
+    <t>91579</t>
+  </si>
+  <si>
+    <t>MGT 101</t>
+  </si>
+  <si>
+    <t>Introduction to Responsible Business Management</t>
+  </si>
+  <si>
+    <t>12:00-12:50P</t>
+  </si>
+  <si>
+    <t>91429</t>
+  </si>
+  <si>
+    <t>MAT 109</t>
+  </si>
+  <si>
+    <t>Precalculus Mathematics</t>
+  </si>
+  <si>
+    <t>11:00-11:50A</t>
+  </si>
+  <si>
+    <t>91728</t>
+  </si>
+  <si>
+    <t>RCC 100 09</t>
+  </si>
+  <si>
+    <t>Only in Florida</t>
+  </si>
+  <si>
+    <t>Taylor Brown</t>
+  </si>
+  <si>
+    <t>R00000003</t>
+  </si>
+  <si>
+    <t>91600</t>
+  </si>
+  <si>
+    <t>PSY 101</t>
+  </si>
+  <si>
+    <t>Introduction to Psychology</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>06:45-09:15P</t>
+  </si>
+  <si>
+    <t>91626</t>
+  </si>
+  <si>
+    <t>PSY 250</t>
+  </si>
+  <si>
+    <t>Statistics &amp; Research Methods 1 w/ Lab</t>
+  </si>
+  <si>
+    <t>11:00-12:50P</t>
+  </si>
+  <si>
+    <t>91537</t>
+  </si>
+  <si>
+    <t>LAT 101</t>
+  </si>
+  <si>
+    <t>Introductory Latin 1</t>
+  </si>
+  <si>
+    <t>91738</t>
+  </si>
+  <si>
+    <t>RCC 100 19</t>
+  </si>
+  <si>
+    <t>Successful Pathways thru Music</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>R00000004</t>
+  </si>
+  <si>
+    <t>MUS, ENV</t>
+  </si>
+  <si>
+    <t>91462</t>
+  </si>
+  <si>
+    <t>MUS 151</t>
+  </si>
+  <si>
+    <t>Theory 1</t>
+  </si>
+  <si>
+    <t>91602</t>
+  </si>
+  <si>
+    <t>BUS 236 3</t>
+  </si>
+  <si>
+    <t>Statistics for Business</t>
+  </si>
+  <si>
+    <t>91583</t>
+  </si>
+  <si>
+    <t>INB 200</t>
+  </si>
+  <si>
+    <t>Intro to Intl Business</t>
+  </si>
+  <si>
+    <t>91720</t>
+  </si>
+  <si>
+    <t>RCC 100 01</t>
+  </si>
+  <si>
+    <t>Cultures: Yoga Mind and Body</t>
+  </si>
+  <si>
+    <t>Victor Howard</t>
+  </si>
+  <si>
+    <t>R00000005</t>
+  </si>
+  <si>
+    <t>BUS, PHI</t>
+  </si>
+  <si>
+    <t>Introduction to International Business</t>
+  </si>
+  <si>
+    <t>Matheus Westphalen</t>
+  </si>
+  <si>
+    <t>R10000006</t>
+  </si>
+  <si>
+    <t>ANT</t>
+  </si>
+  <si>
+    <t>91284</t>
+  </si>
+  <si>
+    <t>ANT 200</t>
+  </si>
+  <si>
+    <t>Cultural Anthropologie</t>
+  </si>
+  <si>
+    <t>91818</t>
+  </si>
+  <si>
+    <t>RCC 100 30</t>
+  </si>
+  <si>
+    <t>Children of the World_CE</t>
+  </si>
+  <si>
+    <t>Michael Labonte</t>
+  </si>
+  <si>
+    <t>R00000007</t>
+  </si>
+  <si>
+    <t>MUS, PHY</t>
+  </si>
+  <si>
+    <t>91731</t>
+  </si>
+  <si>
+    <t>RCC 100 12</t>
+  </si>
+  <si>
+    <t>Electricity &amp; Making for Change</t>
+  </si>
+  <si>
+    <t>Nick Miller</t>
+  </si>
+  <si>
+    <t>R00000008</t>
+  </si>
+  <si>
+    <t>PSY</t>
   </si>
   <si>
     <t>91528</t>
@@ -185,138 +371,6 @@
     <t>Intro to Formal Logic</t>
   </si>
   <si>
-    <t>12:00-12:50P</t>
-  </si>
-  <si>
-    <t>91721</t>
-  </si>
-  <si>
-    <t>RCC 100 02</t>
-  </si>
-  <si>
-    <t>Making Art in the 2D</t>
-  </si>
-  <si>
-    <t>Taylor Brown</t>
-  </si>
-  <si>
-    <t>R00000003</t>
-  </si>
-  <si>
-    <t>91429</t>
-  </si>
-  <si>
-    <t>MAT 109</t>
-  </si>
-  <si>
-    <t>Precalculus Mathematics</t>
-  </si>
-  <si>
-    <t>11:00-11:50A</t>
-  </si>
-  <si>
-    <t>Txt/Context: 10 Amazing Books</t>
-  </si>
-  <si>
-    <t>91462</t>
-  </si>
-  <si>
-    <t>MUS 151</t>
-  </si>
-  <si>
-    <t>Theory 1</t>
-  </si>
-  <si>
-    <t>91731</t>
-  </si>
-  <si>
-    <t>RCC 100 12</t>
-  </si>
-  <si>
-    <t>Electricity &amp; Making for Change</t>
-  </si>
-  <si>
-    <t>09:00-09:50A</t>
-  </si>
-  <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>R00000004</t>
-  </si>
-  <si>
-    <t>MUS, ENV</t>
-  </si>
-  <si>
-    <t>91537</t>
-  </si>
-  <si>
-    <t>LAT 101</t>
-  </si>
-  <si>
-    <t>Introductory Latin 1</t>
-  </si>
-  <si>
-    <t>91720</t>
-  </si>
-  <si>
-    <t>RCC 100 01</t>
-  </si>
-  <si>
-    <t>Cultures: Yoga Mind and Body</t>
-  </si>
-  <si>
-    <t>Victor Howard</t>
-  </si>
-  <si>
-    <t>R00000005</t>
-  </si>
-  <si>
-    <t>BUS, PHI</t>
-  </si>
-  <si>
-    <t>91583</t>
-  </si>
-  <si>
-    <t>INB 200</t>
-  </si>
-  <si>
-    <t>Introduction to International Business</t>
-  </si>
-  <si>
-    <t>Intro to Computer Science</t>
-  </si>
-  <si>
-    <t>Matheus Westphalen</t>
-  </si>
-  <si>
-    <t>R10000006</t>
-  </si>
-  <si>
-    <t>ANT</t>
-  </si>
-  <si>
-    <t>91284</t>
-  </si>
-  <si>
-    <t>ANT 200</t>
-  </si>
-  <si>
-    <t>Cultural Anthropologie</t>
-  </si>
-  <si>
-    <t>91227</t>
-  </si>
-  <si>
-    <t>ECO 221</t>
-  </si>
-  <si>
-    <t>Statistics for Economics</t>
-  </si>
-  <si>
-    <t>02:00-03:15P</t>
-  </si>
-  <si>
     <t>91221</t>
   </si>
   <si>
@@ -324,57 +378,6 @@
   </si>
   <si>
     <t>Mathematical Mths for Econ</t>
-  </si>
-  <si>
-    <t>91818</t>
-  </si>
-  <si>
-    <t>RCC 100 30</t>
-  </si>
-  <si>
-    <t>Children of the World_CE</t>
-  </si>
-  <si>
-    <t>Michael Labonte</t>
-  </si>
-  <si>
-    <t>R00000007</t>
-  </si>
-  <si>
-    <t>MUS, PHY</t>
-  </si>
-  <si>
-    <t>Nick Miller</t>
-  </si>
-  <si>
-    <t>R00000008</t>
-  </si>
-  <si>
-    <t>PSY</t>
-  </si>
-  <si>
-    <t>91600</t>
-  </si>
-  <si>
-    <t>PSY 101</t>
-  </si>
-  <si>
-    <t>Introduction to Psychology</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>06:45-09:15P</t>
-  </si>
-  <si>
-    <t>91602</t>
-  </si>
-  <si>
-    <t>BUS 236 2</t>
-  </si>
-  <si>
-    <t>Statistics for Business</t>
   </si>
 </sst>
 </file>
@@ -884,7 +887,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -892,7 +895,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -900,7 +903,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -925,53 +928,53 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>105</v>
+        <v>56</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>109</v>
+        <v>60</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>109</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>24</v>
@@ -997,10 +1000,10 @@
         <v>24</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>